<commit_message>
Re-organises shortcut sections for easier reference.
</commit_message>
<xml_diff>
--- a/git-terminal-keyboard-shortcuts.xlsx
+++ b/git-terminal-keyboard-shortcuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Smith/GIT/git-keyboard-shortcuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9E14D61-25DA-7042-AC95-5113D5A442F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306629C-44E8-5A4E-BE54-1723B9C9B142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="0" windowWidth="33180" windowHeight="28800" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="55820" yWindow="0" windowWidth="33180" windowHeight="28800" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -8272,9 +8272,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8594,8 +8594,8 @@
   </sheetPr>
   <dimension ref="A1:F349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="212" zoomScaleNormal="210" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="C283" sqref="C283"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="212" zoomScaleNormal="210" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8672,14 +8672,14 @@
       <c r="A8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
@@ -8701,14 +8701,14 @@
       <c r="A12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="10" t="s">
@@ -8859,14 +8859,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="27" thickBot="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6">
       <c r="C27" s="1" t="s">
@@ -8992,14 +8992,14 @@
       <c r="A42" s="21"/>
     </row>
     <row r="43" spans="1:6" ht="27" thickBot="1">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:6">
       <c r="C44" s="1" t="s">
@@ -9074,14 +9074,14 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="27" thickBot="1">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
     </row>
     <row r="55" spans="1:6">
       <c r="C55" s="1" t="s">
@@ -9411,14 +9411,14 @@
       <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:6" ht="27" thickBot="1">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="26"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="27"/>
     </row>
     <row r="89" spans="1:6">
       <c r="C89" s="1" t="s">
@@ -10109,7 +10109,7 @@
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="C143" s="27" t="s">
+      <c r="C143" s="25" t="s">
         <v>366</v>
       </c>
       <c r="D143" s="14" t="s">
@@ -10210,14 +10210,14 @@
       <c r="C150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="27" thickBot="1">
-      <c r="A151" s="25" t="s">
+      <c r="A151" s="26" t="s">
         <v>524</v>
       </c>
-      <c r="B151" s="25"/>
-      <c r="C151" s="25"/>
-      <c r="D151" s="25"/>
-      <c r="E151" s="25"/>
-      <c r="F151" s="25"/>
+      <c r="B151" s="26"/>
+      <c r="C151" s="26"/>
+      <c r="D151" s="26"/>
+      <c r="E151" s="26"/>
+      <c r="F151" s="26"/>
     </row>
     <row r="152" spans="1:6">
       <c r="C152" s="8" t="s">
@@ -10277,7 +10277,7 @@
       </c>
     </row>
     <row r="160" spans="1:6">
-      <c r="C160" s="27" t="s">
+      <c r="C160" s="25" t="s">
         <v>509</v>
       </c>
       <c r="D160" s="14" t="s">
@@ -10605,7 +10605,7 @@
       <c r="C185" s="8"/>
     </row>
     <row r="186" spans="1:6">
-      <c r="C186" s="27" t="s">
+      <c r="C186" s="25" t="s">
         <v>228</v>
       </c>
       <c r="D186" s="14" t="s">
@@ -10735,14 +10735,14 @@
       </c>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="25" t="s">
+      <c r="A196" s="26" t="s">
         <v>525</v>
       </c>
-      <c r="B196" s="25"/>
-      <c r="C196" s="25"/>
-      <c r="D196" s="25"/>
-      <c r="E196" s="25"/>
-      <c r="F196" s="26"/>
+      <c r="B196" s="26"/>
+      <c r="C196" s="26"/>
+      <c r="D196" s="26"/>
+      <c r="E196" s="26"/>
+      <c r="F196" s="27"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="1" t="s">
@@ -11007,14 +11007,14 @@
       <c r="C219" s="2"/>
     </row>
     <row r="221" spans="1:6" ht="27" thickBot="1">
-      <c r="A221" s="25" t="s">
+      <c r="A221" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B221" s="25"/>
-      <c r="C221" s="25"/>
-      <c r="D221" s="25"/>
-      <c r="E221" s="25"/>
-      <c r="F221" s="26"/>
+      <c r="B221" s="26"/>
+      <c r="C221" s="26"/>
+      <c r="D221" s="26"/>
+      <c r="E221" s="26"/>
+      <c r="F221" s="27"/>
     </row>
     <row r="224" spans="1:6">
       <c r="C224" s="1" t="s">
@@ -11541,14 +11541,14 @@
       </c>
     </row>
     <row r="268" spans="1:6" ht="27" thickBot="1">
-      <c r="A268" s="25" t="s">
+      <c r="A268" s="26" t="s">
         <v>526</v>
       </c>
-      <c r="B268" s="25"/>
-      <c r="C268" s="25"/>
-      <c r="D268" s="25"/>
-      <c r="E268" s="25"/>
-      <c r="F268" s="26"/>
+      <c r="B268" s="26"/>
+      <c r="C268" s="26"/>
+      <c r="D268" s="26"/>
+      <c r="E268" s="26"/>
+      <c r="F268" s="27"/>
     </row>
     <row r="269" spans="1:6">
       <c r="C269" s="1" t="s">
@@ -11970,14 +11970,14 @@
       </c>
     </row>
     <row r="312" spans="1:6" ht="27" thickBot="1">
-      <c r="A312" s="25" t="s">
+      <c r="A312" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="B312" s="25"/>
-      <c r="C312" s="25"/>
-      <c r="D312" s="25"/>
-      <c r="E312" s="25"/>
-      <c r="F312" s="26"/>
+      <c r="B312" s="26"/>
+      <c r="C312" s="26"/>
+      <c r="D312" s="26"/>
+      <c r="E312" s="26"/>
+      <c r="F312" s="27"/>
     </row>
     <row r="313" spans="1:6">
       <c r="C313" s="1" t="s">
@@ -12111,14 +12111,14 @@
       </c>
     </row>
     <row r="333" spans="1:6" ht="27" thickBot="1">
-      <c r="A333" s="25" t="s">
+      <c r="A333" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B333" s="25"/>
-      <c r="C333" s="25"/>
-      <c r="D333" s="25"/>
-      <c r="E333" s="25"/>
-      <c r="F333" s="26"/>
+      <c r="B333" s="26"/>
+      <c r="C333" s="26"/>
+      <c r="D333" s="26"/>
+      <c r="E333" s="26"/>
+      <c r="F333" s="27"/>
     </row>
     <row r="335" spans="1:6">
       <c r="C335" s="1" t="s">
@@ -12302,11 +12302,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A333:F333"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A312:F312"/>
     <mergeCell ref="A268:F268"/>
@@ -12314,6 +12309,11 @@
     <mergeCell ref="A196:F196"/>
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A151:F151"/>
+    <mergeCell ref="A333:F333"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A26:F26"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Final changes for Sunday 9th January.
</commit_message>
<xml_diff>
--- a/git-terminal-keyboard-shortcuts.xlsx
+++ b/git-terminal-keyboard-shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Smith/GIT/git-keyboard-shortcuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306629C-44E8-5A4E-BE54-1723B9C9B142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1518D36-518F-B946-A4DC-9682963E13E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="55820" yWindow="0" windowWidth="33180" windowHeight="28800" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
@@ -12302,6 +12302,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A333:F333"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A312:F312"/>
     <mergeCell ref="A268:F268"/>
@@ -12309,11 +12314,6 @@
     <mergeCell ref="A196:F196"/>
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A151:F151"/>
-    <mergeCell ref="A333:F333"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A26:F26"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
These changes to formating and clarification were done on 2021/01/12.
</commit_message>
<xml_diff>
--- a/git-terminal-keyboard-shortcuts.xlsx
+++ b/git-terminal-keyboard-shortcuts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eyvind-earle/Dropbox/localhost-backup/GIT/steveos-git-shortcuts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Smith/GIT/steveos-git-shortcuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1379619-CCE0-004E-B90A-199F7238C58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B267EEE-7688-044A-B4DA-1AB9E6E4D2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="0" windowWidth="32820" windowHeight="28800" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="15080" yWindow="0" windowWidth="32820" windowHeight="28800" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="582">
   <si>
     <t>Configuration</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>ls</t>
-  </si>
-  <si>
-    <t>ls -la</t>
   </si>
   <si>
     <t>cd</t>
@@ -9138,6 +9135,52 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of the point of divergence of the branches</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls (-la </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo Italic"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> -a)</t>
+    </r>
+  </si>
+  <si>
+    <t>Restore file changes from working file to original state</t>
+  </si>
+  <si>
+    <r>
+      <t>Revert changes made in a commit (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Menlo Bold Italic"/>
+      </rPr>
+      <t>SHA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -9145,7 +9188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41">
+  <fonts count="43">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9387,6 +9430,21 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -9435,7 +9493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9464,13 +9522,15 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9790,8 +9850,8 @@
   </sheetPr>
   <dimension ref="A1:G366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScale="212" zoomScaleNormal="210" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="A337" sqref="A337:F337"/>
+    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="212" zoomScaleNormal="210" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C207" sqref="C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9806,117 +9866,117 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31">
       <c r="A1" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
+      <c r="A9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -9925,12 +9985,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -9939,12 +9999,12 @@
         <v>2</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="C17" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>5</v>
@@ -9953,7 +10013,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -9964,10 +10024,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -9978,10 +10038,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -9992,10 +10052,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>519</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -10006,10 +10066,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>521</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -10020,10 +10080,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -10034,10 +10094,10 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -10048,10 +10108,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -10062,10 +10122,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>557</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -10079,7 +10139,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -10090,828 +10150,828 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="27" thickBot="1">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" spans="1:6">
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="C31" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="C32" s="1" t="s">
-        <v>10</v>
+        <v>579</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="C34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="C36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="C37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="C39" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="C40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="C41" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="C42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="C44" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="21"/>
     </row>
     <row r="46" spans="1:6" ht="27" thickBot="1">
-      <c r="A46" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27"/>
+      <c r="A46" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="32"/>
     </row>
     <row r="47" spans="1:6">
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="C48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="C49" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="C50" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="C51" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="C52" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="C53" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="C54" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="C55" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="27" thickBot="1">
-      <c r="A57" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
+      <c r="A57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
     </row>
     <row r="58" spans="1:6">
       <c r="C58" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="C59" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="C60" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="C61" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="C62" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="C63" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="C64" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="C65" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="C66" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="C67" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="C68" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="C69" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="C70" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="C72" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F72" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="C73" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="C75" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D75" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F75" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="C83" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D83" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F83" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F88" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F89" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:6" ht="27" thickBot="1">
-      <c r="A91" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="27"/>
+      <c r="A91" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="32"/>
     </row>
     <row r="92" spans="1:6">
       <c r="C92" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="C94" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F94" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F95" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F96" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F101" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F102" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F106" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F107" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F109" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F110" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F111" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="C113" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>5</v>
@@ -10920,12 +10980,12 @@
         <v>1</v>
       </c>
       <c r="F113" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="C114" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>5</v>
@@ -10934,26 +10994,26 @@
         <v>1</v>
       </c>
       <c r="F114" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="C115" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F115" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="C116" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>5</v>
@@ -10962,35 +11022,35 @@
         <v>1</v>
       </c>
       <c r="F116" s="23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="C117" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F117" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="C118" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F118" s="16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -11001,10 +11061,10 @@
         <v>4</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F119" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -11015,10 +11075,10 @@
         <v>4</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F120" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -11029,10 +11089,10 @@
         <v>4</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F121" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -11043,10 +11103,10 @@
         <v>4</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F122" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -11057,10 +11117,10 @@
         <v>4</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F123" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -11071,10 +11131,10 @@
         <v>4</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F124" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -11085,10 +11145,10 @@
         <v>4</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F125" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -11099,10 +11159,10 @@
         <v>4</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F126" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -11113,10 +11173,10 @@
         <v>4</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F127" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -11127,10 +11187,10 @@
         <v>4</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F128" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -11141,10 +11201,10 @@
         <v>4</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F129" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -11155,10 +11215,10 @@
         <v>4</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F130" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -11169,10 +11229,10 @@
         <v>4</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F131" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -11183,10 +11243,10 @@
         <v>4</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F132" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -11197,10 +11257,10 @@
         <v>4</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F133" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -11211,10 +11271,10 @@
         <v>4</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F134" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -11225,10 +11285,10 @@
         <v>4</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F135" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -11239,122 +11299,122 @@
         <v>4</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F136" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D138" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E138" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="F138" s="22" t="s">
         <v>451</v>
-      </c>
-      <c r="F138" s="22" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F139" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F140" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F141" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F142" s="15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="C144" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F144" s="23" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="C145" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="D145" s="28" t="s">
+      <c r="C145" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="D145" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E145" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F145" s="30" t="s">
-        <v>524</v>
+      <c r="E145" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F145" s="28" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="C146" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F146" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -11365,10 +11425,10 @@
         <v>4</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F147" s="15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -11379,10 +11439,10 @@
         <v>4</v>
       </c>
       <c r="C148" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F148" s="15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -11393,10 +11453,10 @@
         <v>4</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F149" s="15" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -11407,10 +11467,10 @@
         <v>4</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F150" s="15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -11421,10 +11481,10 @@
         <v>4</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F151" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -11435,31 +11495,31 @@
         <v>4</v>
       </c>
       <c r="C152" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="F152" s="15" t="s">
         <v>531</v>
-      </c>
-      <c r="F152" s="15" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="153" spans="1:6">
       <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:6" ht="27" thickBot="1">
-      <c r="A154" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="B154" s="26"/>
-      <c r="C154" s="26"/>
-      <c r="D154" s="26"/>
-      <c r="E154" s="26"/>
-      <c r="F154" s="26"/>
+      <c r="A154" s="31" t="s">
+        <v>458</v>
+      </c>
+      <c r="B154" s="31"/>
+      <c r="C154" s="31"/>
+      <c r="D154" s="31"/>
+      <c r="E154" s="31"/>
+      <c r="F154" s="31"/>
     </row>
     <row r="155" spans="1:6">
       <c r="C155" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="F155" s="31" t="s">
-        <v>533</v>
+        <v>276</v>
+      </c>
+      <c r="F155" s="29" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -11467,44 +11527,44 @@
     </row>
     <row r="157" spans="1:6">
       <c r="C157" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D157" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E157" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F157" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F158" s="15" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F159" s="15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -11512,164 +11572,164 @@
     </row>
     <row r="161" spans="1:6">
       <c r="C161" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D161" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E161" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F161" s="22" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F162" s="15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F163" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F164" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F165" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F166" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C167" s="25" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D167" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F167" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F168" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F169" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -11677,77 +11737,77 @@
     </row>
     <row r="171" spans="1:6">
       <c r="C171" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D171" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F171" s="22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F172" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F173" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F174" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F175" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="177" spans="1:6">
       <c r="C177" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D177" s="14" t="s">
         <v>5</v>
@@ -11756,7 +11816,7 @@
         <v>1</v>
       </c>
       <c r="F177" s="22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -11767,10 +11827,10 @@
         <v>4</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F178" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -11781,10 +11841,10 @@
         <v>4</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F179" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -11795,10 +11855,10 @@
         <v>4</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F180" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -11809,10 +11869,10 @@
         <v>4</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F181" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -11823,10 +11883,10 @@
         <v>4</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F182" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -11837,10 +11897,10 @@
         <v>4</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F183" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -11851,10 +11911,10 @@
         <v>4</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F184" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -11865,10 +11925,10 @@
         <v>4</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F185" s="15" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -11879,10 +11939,10 @@
         <v>4</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F186" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -11893,10 +11953,10 @@
         <v>4</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F187" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -11907,10 +11967,10 @@
         <v>4</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F188" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -11918,346 +11978,346 @@
     </row>
     <row r="190" spans="1:6">
       <c r="C190" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D190" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E190" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F190" s="16"/>
     </row>
     <row r="191" spans="1:6">
       <c r="A191" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C191" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F191" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="192" spans="1:6">
       <c r="A192" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F192" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F193" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="194" spans="1:6">
       <c r="A194" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F194" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="A195" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C195" s="24" t="s">
         <v>211</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C195" s="24" t="s">
-        <v>212</v>
       </c>
       <c r="D195" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E195" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F195" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F196" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F197" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F198" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="27" thickBot="1">
-      <c r="A200" s="26" t="s">
-        <v>553</v>
-      </c>
-      <c r="B200" s="26"/>
-      <c r="C200" s="26"/>
-      <c r="D200" s="26"/>
-      <c r="E200" s="26"/>
-      <c r="F200" s="27"/>
+      <c r="A200" s="31" t="s">
+        <v>552</v>
+      </c>
+      <c r="B200" s="31"/>
+      <c r="C200" s="31"/>
+      <c r="D200" s="31"/>
+      <c r="E200" s="31"/>
+      <c r="F200" s="32"/>
     </row>
     <row r="201" spans="1:6">
       <c r="C201" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F201" s="15" t="s">
-        <v>36</v>
+        <v>581</v>
       </c>
     </row>
     <row r="202" spans="1:6">
       <c r="C202" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F202" s="15" t="s">
-        <v>310</v>
+        <v>580</v>
       </c>
     </row>
     <row r="203" spans="1:6">
       <c r="C203" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F203" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="204" spans="1:6">
       <c r="C204" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F204" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="207" spans="1:6">
       <c r="C207" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F207" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="208" spans="1:6">
       <c r="C208" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F208" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C209" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B209" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="F209" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F210" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F211" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F213" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C214" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F214" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="F214" s="15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F215" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F216" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F217" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="218" spans="1:6">
       <c r="A218" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F218" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -12268,10 +12328,10 @@
         <v>4</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F219" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -12282,10 +12342,10 @@
         <v>4</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F220" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -12296,10 +12356,10 @@
         <v>4</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F221" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -12309,493 +12369,493 @@
       <c r="C223" s="2"/>
     </row>
     <row r="225" spans="1:6" ht="27" thickBot="1">
-      <c r="A225" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B225" s="26"/>
-      <c r="C225" s="26"/>
-      <c r="D225" s="26"/>
-      <c r="E225" s="26"/>
-      <c r="F225" s="27"/>
+      <c r="A225" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B225" s="31"/>
+      <c r="C225" s="31"/>
+      <c r="D225" s="31"/>
+      <c r="E225" s="31"/>
+      <c r="F225" s="32"/>
     </row>
     <row r="228" spans="1:6">
       <c r="C228" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D228" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F228" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="229" spans="1:6">
       <c r="C229" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F229" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="230" spans="1:6">
       <c r="C230" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F230" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="231" spans="1:6">
       <c r="C231" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F231" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C232" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F232" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="F232" s="15" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C233" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F233" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="F233" s="15" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F234" s="15" t="s">
         <v>75</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C234" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F234" s="15" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C235" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F235" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="F235" s="15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F236" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F237" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C238" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F238" s="15" t="s">
         <v>192</v>
-      </c>
-      <c r="F238" s="15" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F239" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F240" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F241" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="242" spans="1:6">
       <c r="C242" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F242" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F243" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F244" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="245" spans="1:6">
       <c r="A245" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F245" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F246" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F247" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F248" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F249" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C250" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F250" s="15" t="s">
         <v>263</v>
-      </c>
-      <c r="F250" s="15" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="252" spans="1:6">
       <c r="C252" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F252" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C253" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C253" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="F253" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="254" spans="1:6">
       <c r="A254" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F254" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F255" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F256" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="257" spans="1:6">
       <c r="A257" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F257" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="258" spans="1:6">
       <c r="A258" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F258" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="259" spans="1:6">
       <c r="A259" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F259" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="260" spans="1:6">
       <c r="A260" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C260" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F260" s="15" t="s">
         <v>263</v>
-      </c>
-      <c r="F260" s="15" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="261" spans="1:6">
       <c r="C261" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F261" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="F261" s="15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="262" spans="1:6">
       <c r="C262" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F262" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="264" spans="1:6">
       <c r="C264" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F264" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="267" spans="1:6">
       <c r="C267" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F267" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="268" spans="1:6">
@@ -12806,10 +12866,10 @@
         <v>4</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F268" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" spans="1:6">
@@ -12820,10 +12880,10 @@
         <v>4</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F269" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" spans="1:6">
@@ -12834,125 +12894,125 @@
         <v>4</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D270" s="9"/>
       <c r="E270" s="9"/>
       <c r="F270" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="27" thickBot="1">
-      <c r="A272" s="26" t="s">
-        <v>460</v>
-      </c>
-      <c r="B272" s="26"/>
-      <c r="C272" s="26"/>
-      <c r="D272" s="26"/>
-      <c r="E272" s="26"/>
-      <c r="F272" s="27"/>
+      <c r="A272" s="31" t="s">
+        <v>459</v>
+      </c>
+      <c r="B272" s="31"/>
+      <c r="C272" s="31"/>
+      <c r="D272" s="31"/>
+      <c r="E272" s="31"/>
+      <c r="F272" s="32"/>
     </row>
     <row r="273" spans="1:6">
       <c r="C273" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E273" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F273" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="F273" s="15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="274" spans="1:6">
       <c r="A274" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C274" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F274" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="F274" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="275" spans="1:6">
       <c r="A275" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F275" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="276" spans="1:6">
       <c r="A276" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F276" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="277" spans="1:6">
       <c r="A277" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F277" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="278" spans="1:6">
       <c r="A278" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F278" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="279" spans="1:6">
       <c r="A279" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F279" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="281" spans="1:6">
       <c r="C281" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>5</v>
@@ -12961,7 +13021,7 @@
         <v>3</v>
       </c>
       <c r="F281" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="282" spans="1:6">
@@ -12972,10 +13032,10 @@
         <v>4</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F282" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="283" spans="1:6">
@@ -12986,10 +13046,10 @@
         <v>4</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F283" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="284" spans="1:6">
@@ -13000,10 +13060,10 @@
         <v>4</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F284" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="285" spans="1:6">
@@ -13014,10 +13074,10 @@
         <v>4</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F285" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="286" spans="1:6">
@@ -13028,10 +13088,10 @@
         <v>4</v>
       </c>
       <c r="C286" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F286" s="15" t="s">
         <v>231</v>
-      </c>
-      <c r="F286" s="15" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="287" spans="1:6">
@@ -13042,10 +13102,10 @@
         <v>4</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F287" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="288" spans="1:6">
@@ -13056,10 +13116,10 @@
         <v>4</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F288" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="289" spans="1:6">
@@ -13070,10 +13130,10 @@
         <v>4</v>
       </c>
       <c r="C289" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F289" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="F289" s="15" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="290" spans="1:6">
@@ -13084,10 +13144,10 @@
         <v>4</v>
       </c>
       <c r="C290" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F290" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="F290" s="15" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="291" spans="1:6">
@@ -13098,10 +13158,10 @@
         <v>4</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F291" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="292" spans="1:6">
@@ -13112,42 +13172,42 @@
         <v>4</v>
       </c>
       <c r="C292" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F292" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="F292" s="15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="297" spans="1:6">
       <c r="C297" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F297" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="298" spans="1:6">
       <c r="C298" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F298" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="299" spans="1:6">
       <c r="C299" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F299" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="300" spans="1:6">
       <c r="C300" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F300" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="301" spans="1:6">
@@ -13155,369 +13215,369 @@
     </row>
     <row r="302" spans="1:6">
       <c r="C302" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F302" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="303" spans="1:6">
       <c r="C303" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F303" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="F303" s="15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="305" spans="1:6">
       <c r="C305" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F305" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:6">
       <c r="C306" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F306" s="15" t="s">
         <v>228</v>
-      </c>
-      <c r="F306" s="15" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="307" spans="1:6">
       <c r="C307" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F307" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="308" spans="1:6">
       <c r="C308" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F308" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="309" spans="1:6">
       <c r="C309" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D309" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E309" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F309" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="310" spans="1:6">
       <c r="A310" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F310" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="311" spans="1:6">
       <c r="A311" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F311" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="312" spans="1:6">
       <c r="A312" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F312" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="313" spans="1:6">
       <c r="A313" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F313" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="316" spans="1:6" ht="27" thickBot="1">
-      <c r="A316" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="B316" s="26"/>
-      <c r="C316" s="26"/>
-      <c r="D316" s="26"/>
-      <c r="E316" s="26"/>
-      <c r="F316" s="27"/>
+      <c r="A316" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="B316" s="31"/>
+      <c r="C316" s="31"/>
+      <c r="D316" s="31"/>
+      <c r="E316" s="31"/>
+      <c r="F316" s="32"/>
     </row>
     <row r="317" spans="1:6">
       <c r="C317" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D317" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E317" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F317" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="F317" s="15" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="318" spans="1:6">
       <c r="C318" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F318" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="319" spans="1:6">
       <c r="C319" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F319" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="320" spans="1:6">
       <c r="C320" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F320" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="321" spans="3:6">
       <c r="C321" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F321" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="322" spans="3:6">
       <c r="C322" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F322" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="323" spans="3:6">
       <c r="C323" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F323" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="324" spans="3:6">
       <c r="C324" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F324" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="325" spans="3:6">
       <c r="C325" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F325" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="326" spans="3:6">
       <c r="C326" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F326" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="F326" s="15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="327" spans="3:6">
       <c r="C327" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F327" s="15" t="s">
         <v>257</v>
-      </c>
-      <c r="F327" s="15" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="329" spans="3:6">
       <c r="C329" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F329" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="F329" s="15" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="330" spans="3:6">
       <c r="C330" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F330" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="F330" s="15" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="331" spans="3:6">
       <c r="C331" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F331" s="15" t="s">
         <v>271</v>
-      </c>
-      <c r="F331" s="15" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="332" spans="3:6">
       <c r="C332" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F332" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="F332" s="15" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="334" spans="3:6">
       <c r="C334" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="337" spans="1:6" ht="27" thickBot="1">
-      <c r="A337" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="B337" s="26"/>
-      <c r="C337" s="26"/>
-      <c r="D337" s="26"/>
-      <c r="E337" s="26"/>
-      <c r="F337" s="27"/>
+      <c r="A337" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="B337" s="31"/>
+      <c r="C337" s="31"/>
+      <c r="D337" s="31"/>
+      <c r="E337" s="31"/>
+      <c r="F337" s="32"/>
     </row>
     <row r="338" spans="1:6">
       <c r="C338" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F338" s="15" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="339" spans="1:6">
-      <c r="C339" s="28"/>
-      <c r="D339" s="28"/>
-      <c r="E339" s="28"/>
-      <c r="F339" s="30"/>
+      <c r="C339" s="26"/>
+      <c r="D339" s="26"/>
+      <c r="E339" s="26"/>
+      <c r="F339" s="28"/>
     </row>
     <row r="340" spans="1:6">
       <c r="C340" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D340" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E340" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F340" s="22" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="341" spans="1:6">
       <c r="A341" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F341" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="343" spans="1:6">
       <c r="C343" s="14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D343" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E343" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F343" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="344" spans="1:6">
       <c r="A344" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C344" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F344" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="346" spans="1:6">
       <c r="C346" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D346" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F346" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="347" spans="1:6">
       <c r="C347" s="14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D347" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E347" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F347" s="22" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -13528,10 +13588,10 @@
         <v>4</v>
       </c>
       <c r="C348" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F348" s="15" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="349" spans="1:6">
@@ -13542,10 +13602,10 @@
         <v>4</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F349" s="15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="350" spans="1:6">
@@ -13556,10 +13616,10 @@
         <v>4</v>
       </c>
       <c r="C350" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F350" s="15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="351" spans="1:6">
@@ -13570,10 +13630,10 @@
         <v>4</v>
       </c>
       <c r="C351" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F351" s="15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -13584,10 +13644,10 @@
         <v>4</v>
       </c>
       <c r="C352" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F352" s="15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -13598,10 +13658,10 @@
         <v>4</v>
       </c>
       <c r="C353" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="F353" s="15" t="s">
         <v>569</v>
-      </c>
-      <c r="F353" s="15" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -13612,10 +13672,10 @@
         <v>4</v>
       </c>
       <c r="C354" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F354" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -13626,10 +13686,10 @@
         <v>4</v>
       </c>
       <c r="C355" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F355" s="15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -13640,10 +13700,10 @@
         <v>4</v>
       </c>
       <c r="C356" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F356" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -13651,71 +13711,71 @@
     </row>
     <row r="358" spans="1:7">
       <c r="C358" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D358" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E358" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F358" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="359" spans="1:7">
       <c r="A359" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F359" s="15" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="360" spans="1:7">
       <c r="A360" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F360" s="15" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="361" spans="1:7">
       <c r="A361" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B361" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F361" s="15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="363" spans="1:7">
-      <c r="G363" s="32"/>
+      <c r="G363" s="30"/>
     </row>
     <row r="364" spans="1:7">
-      <c r="G364" s="32"/>
+      <c r="G364" s="30"/>
     </row>
     <row r="365" spans="1:7">
-      <c r="G365" s="32"/>
+      <c r="G365" s="30"/>
     </row>
     <row r="366" spans="1:7">
-      <c r="G366" s="32"/>
+      <c r="G366" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>